<commit_message>
version finale article: 21_08_23
</commit_message>
<xml_diff>
--- a/result/cq/instances.xlsx
+++ b/result/cq/instances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliwa/Documents/Ulaval/thesis/works/cimentQuebec/result/cq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36599063-D949-5B4A-9804-69728984151B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F15BD90-FA17-074F-ADDE-0B73A0D977C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18280" yWindow="740" windowWidth="11960" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instances" sheetId="1" r:id="rId1"/>
@@ -1702,8 +1702,8 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1773,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="14" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E2,"#"),"_",TEXT(C2,"#"),"_",TEXT(D2,"#"),"_",TEXT(B2,"#"))</f>
+        <f t="shared" ref="H2:H33" si="0">_xlfn.CONCAT("C","_",TEXT(E2,"#"),"_",TEXT(C2,"#"),"_",TEXT(D2,"#"),"_",TEXT(B2,"#"))</f>
         <v>C_13_11_12_1</v>
       </c>
       <c r="I2" s="14" t="str">
@@ -1807,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E3,"#"),"_",TEXT(C3,"#"),"_",TEXT(D3,"#"),"_",TEXT(B3,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_13_5_8_1</v>
       </c>
       <c r="I3" s="3" t="str">
@@ -1841,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E4,"#"),"_",TEXT(C4,"#"),"_",TEXT(D4,"#"),"_",TEXT(B4,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_18_6_11_2</v>
       </c>
       <c r="I4" s="3" t="str">
@@ -1875,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E5,"#"),"_",TEXT(C5,"#"),"_",TEXT(D5,"#"),"_",TEXT(B5,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_15_4_7_2</v>
       </c>
       <c r="I5" s="3" t="str">
@@ -1909,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E6,"#"),"_",TEXT(C6,"#"),"_",TEXT(D6,"#"),"_",TEXT(B6,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_19_7_8_2</v>
       </c>
       <c r="I6" s="3" t="str">
@@ -1943,7 +1943,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E7,"#"),"_",TEXT(C7,"#"),"_",TEXT(D7,"#"),"_",TEXT(B7,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_29_10_14_3</v>
       </c>
       <c r="I7" s="3" t="str">
@@ -1977,7 +1977,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E8,"#"),"_",TEXT(C8,"#"),"_",TEXT(D8,"#"),"_",TEXT(B8,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_31_8_11_3</v>
       </c>
       <c r="I8" s="3" t="str">
@@ -2011,7 +2011,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E9,"#"),"_",TEXT(C9,"#"),"_",TEXT(D9,"#"),"_",TEXT(B9,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_28_6_6_2</v>
       </c>
       <c r="I9" s="3" t="str">
@@ -2045,7 +2045,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E10,"#"),"_",TEXT(C10,"#"),"_",TEXT(D10,"#"),"_",TEXT(B10,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_35_9_10_3</v>
       </c>
       <c r="I10" s="3" t="str">
@@ -2079,7 +2079,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E11,"#"),"_",TEXT(C11,"#"),"_",TEXT(D11,"#"),"_",TEXT(B11,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_76_40_43_6</v>
       </c>
       <c r="I11" s="3" t="str">
@@ -2113,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E12,"#"),"_",TEXT(C12,"#"),"_",TEXT(D12,"#"),"_",TEXT(B12,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_104_42_47_8</v>
       </c>
       <c r="I12" s="3" t="str">
@@ -2147,7 +2147,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E13,"#"),"_",TEXT(C13,"#"),"_",TEXT(D13,"#"),"_",TEXT(B13,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_94_63_70_7</v>
       </c>
       <c r="I13" s="3" t="str">
@@ -2181,7 +2181,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E14,"#"),"_",TEXT(C14,"#"),"_",TEXT(D14,"#"),"_",TEXT(B14,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_116_67_78_8</v>
       </c>
       <c r="I14" s="3" t="str">
@@ -2215,7 +2215,7 @@
         <v>2</v>
       </c>
       <c r="H15" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E15,"#"),"_",TEXT(C15,"#"),"_",TEXT(D15,"#"),"_",TEXT(B15,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_116_71_82_8</v>
       </c>
       <c r="I15" s="3" t="str">
@@ -2249,7 +2249,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E16,"#"),"_",TEXT(C16,"#"),"_",TEXT(D16,"#"),"_",TEXT(B16,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_117_57_70_6</v>
       </c>
       <c r="I16" s="3" t="str">
@@ -2283,7 +2283,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E17,"#"),"_",TEXT(C17,"#"),"_",TEXT(D17,"#"),"_",TEXT(B17,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_137_79_83_7</v>
       </c>
       <c r="I17" s="3" t="str">
@@ -2317,7 +2317,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E18,"#"),"_",TEXT(C18,"#"),"_",TEXT(D18,"#"),"_",TEXT(B18,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_127_66_80_8</v>
       </c>
       <c r="I18" s="3" t="str">
@@ -2351,7 +2351,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E19,"#"),"_",TEXT(C19,"#"),"_",TEXT(D19,"#"),"_",TEXT(B19,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_128_68_74_7</v>
       </c>
       <c r="I19" s="3" t="str">
@@ -2385,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="H20" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E20,"#"),"_",TEXT(C20,"#"),"_",TEXT(D20,"#"),"_",TEXT(B20,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_136_85_97_8</v>
       </c>
       <c r="I20" s="3" t="str">
@@ -2419,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E21,"#"),"_",TEXT(C21,"#"),"_",TEXT(D21,"#"),"_",TEXT(B21,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_128_78_85_8</v>
       </c>
       <c r="I21" s="3" t="str">
@@ -2453,7 +2453,7 @@
         <v>2</v>
       </c>
       <c r="H22" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E22,"#"),"_",TEXT(C22,"#"),"_",TEXT(D22,"#"),"_",TEXT(B22,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_131_77_85_8</v>
       </c>
       <c r="I22" s="3" t="str">
@@ -2487,7 +2487,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E23,"#"),"_",TEXT(C23,"#"),"_",TEXT(D23,"#"),"_",TEXT(B23,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_137_89_97_7</v>
       </c>
       <c r="I23" s="3" t="str">
@@ -2521,7 +2521,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E24,"#"),"_",TEXT(C24,"#"),"_",TEXT(D24,"#"),"_",TEXT(B24,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_133_84_98_7</v>
       </c>
       <c r="I24" s="3" t="str">
@@ -2555,7 +2555,7 @@
         <v>2</v>
       </c>
       <c r="H25" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E25,"#"),"_",TEXT(C25,"#"),"_",TEXT(D25,"#"),"_",TEXT(B25,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_137_94_107_8</v>
       </c>
       <c r="I25" s="3" t="str">
@@ -2589,7 +2589,7 @@
         <v>2</v>
       </c>
       <c r="H26" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E26,"#"),"_",TEXT(C26,"#"),"_",TEXT(D26,"#"),"_",TEXT(B26,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_132_98_109_8</v>
       </c>
       <c r="I26" s="3" t="str">
@@ -2623,7 +2623,7 @@
         <v>2</v>
       </c>
       <c r="H27" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E27,"#"),"_",TEXT(C27,"#"),"_",TEXT(D27,"#"),"_",TEXT(B27,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_147_115_128_7</v>
       </c>
       <c r="I27" s="3" t="str">
@@ -2657,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="H28" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E28,"#"),"_",TEXT(C28,"#"),"_",TEXT(D28,"#"),"_",TEXT(B28,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_137_79_93_7</v>
       </c>
       <c r="I28" s="3" t="str">
@@ -2691,7 +2691,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E29,"#"),"_",TEXT(C29,"#"),"_",TEXT(D29,"#"),"_",TEXT(B29,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_131_102_117_7</v>
       </c>
       <c r="I29" s="3" t="str">
@@ -2725,7 +2725,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E30,"#"),"_",TEXT(C30,"#"),"_",TEXT(D30,"#"),"_",TEXT(B30,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_116_84_90_8</v>
       </c>
       <c r="I30" s="3" t="str">
@@ -2759,7 +2759,7 @@
         <v>2</v>
       </c>
       <c r="H31" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E31,"#"),"_",TEXT(C31,"#"),"_",TEXT(D31,"#"),"_",TEXT(B31,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_129_101_119_8</v>
       </c>
       <c r="I31" s="3" t="str">
@@ -2793,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="H32" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E32,"#"),"_",TEXT(C32,"#"),"_",TEXT(D32,"#"),"_",TEXT(B32,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_140_106_122_7</v>
       </c>
       <c r="I32" s="3" t="str">
@@ -2827,7 +2827,7 @@
         <v>2</v>
       </c>
       <c r="H33" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E33,"#"),"_",TEXT(C33,"#"),"_",TEXT(D33,"#"),"_",TEXT(B33,"#"))</f>
+        <f t="shared" si="0"/>
         <v>C_141_114_136_8</v>
       </c>
       <c r="I33" s="3" t="str">
@@ -2861,7 +2861,7 @@
         <v>2</v>
       </c>
       <c r="H34" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E34,"#"),"_",TEXT(C34,"#"),"_",TEXT(D34,"#"),"_",TEXT(B34,"#"))</f>
+        <f t="shared" ref="H34:H52" si="1">_xlfn.CONCAT("C","_",TEXT(E34,"#"),"_",TEXT(C34,"#"),"_",TEXT(D34,"#"),"_",TEXT(B34,"#"))</f>
         <v>C_140_114_132_8</v>
       </c>
       <c r="I34" s="3" t="str">
@@ -2895,7 +2895,7 @@
         <v>2</v>
       </c>
       <c r="H35" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E35,"#"),"_",TEXT(C35,"#"),"_",TEXT(D35,"#"),"_",TEXT(B35,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_148_111_127_8</v>
       </c>
       <c r="I35" s="3" t="str">
@@ -2929,7 +2929,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E36,"#"),"_",TEXT(C36,"#"),"_",TEXT(D36,"#"),"_",TEXT(B36,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_143_101_123_8</v>
       </c>
       <c r="I36" s="3" t="str">
@@ -2963,7 +2963,7 @@
         <v>2</v>
       </c>
       <c r="H37" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E37,"#"),"_",TEXT(C37,"#"),"_",TEXT(D37,"#"),"_",TEXT(B37,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_141_109_126_8</v>
       </c>
       <c r="I37" s="3" t="str">
@@ -2997,7 +2997,7 @@
         <v>2</v>
       </c>
       <c r="H38" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E38,"#"),"_",TEXT(C38,"#"),"_",TEXT(D38,"#"),"_",TEXT(B38,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_137_112_129_8</v>
       </c>
       <c r="I38" s="3" t="str">
@@ -3031,7 +3031,7 @@
         <v>2</v>
       </c>
       <c r="H39" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E39,"#"),"_",TEXT(C39,"#"),"_",TEXT(D39,"#"),"_",TEXT(B39,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_142_114_129_8</v>
       </c>
       <c r="I39" s="3" t="str">
@@ -3065,7 +3065,7 @@
         <v>2</v>
       </c>
       <c r="H40" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E40,"#"),"_",TEXT(C40,"#"),"_",TEXT(D40,"#"),"_",TEXT(B40,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_149_98_122_8</v>
       </c>
       <c r="I40" s="3" t="str">
@@ -3099,7 +3099,7 @@
         <v>2</v>
       </c>
       <c r="H41" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E41,"#"),"_",TEXT(C41,"#"),"_",TEXT(D41,"#"),"_",TEXT(B41,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_139_98_108_8</v>
       </c>
       <c r="I41" s="3" t="str">
@@ -3133,7 +3133,7 @@
         <v>2</v>
       </c>
       <c r="H42" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E42,"#"),"_",TEXT(C42,"#"),"_",TEXT(D42,"#"),"_",TEXT(B42,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_154_100_116_8</v>
       </c>
       <c r="I42" s="3" t="str">
@@ -3167,7 +3167,7 @@
         <v>2</v>
       </c>
       <c r="H43" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E43,"#"),"_",TEXT(C43,"#"),"_",TEXT(D43,"#"),"_",TEXT(B43,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_144_108_122_8</v>
       </c>
       <c r="I43" s="3" t="str">
@@ -3201,7 +3201,7 @@
         <v>2</v>
       </c>
       <c r="H44" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E44,"#"),"_",TEXT(C44,"#"),"_",TEXT(D44,"#"),"_",TEXT(B44,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_142_92_107_8</v>
       </c>
       <c r="I44" s="3" t="str">
@@ -3235,7 +3235,7 @@
         <v>2</v>
       </c>
       <c r="H45" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E45,"#"),"_",TEXT(C45,"#"),"_",TEXT(D45,"#"),"_",TEXT(B45,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_138_114_136_8</v>
       </c>
       <c r="I45" s="3" t="str">
@@ -3269,7 +3269,7 @@
         <v>2</v>
       </c>
       <c r="H46" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E46,"#"),"_",TEXT(C46,"#"),"_",TEXT(D46,"#"),"_",TEXT(B46,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_145_116_130_8</v>
       </c>
       <c r="I46" s="3" t="str">
@@ -3303,7 +3303,7 @@
         <v>2</v>
       </c>
       <c r="H47" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E47,"#"),"_",TEXT(C47,"#"),"_",TEXT(D47,"#"),"_",TEXT(B47,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_150_127_136_8</v>
       </c>
       <c r="I47" s="3" t="str">
@@ -3337,7 +3337,7 @@
         <v>2</v>
       </c>
       <c r="H48" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E48,"#"),"_",TEXT(C48,"#"),"_",TEXT(D48,"#"),"_",TEXT(B48,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_148_112_131_8</v>
       </c>
       <c r="I48" s="3" t="str">
@@ -3371,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="H49" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E49,"#"),"_",TEXT(C49,"#"),"_",TEXT(D49,"#"),"_",TEXT(B49,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_144_93_112_8</v>
       </c>
       <c r="I49" s="3" t="str">
@@ -3405,7 +3405,7 @@
         <v>2</v>
       </c>
       <c r="H50" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E50,"#"),"_",TEXT(C50,"#"),"_",TEXT(D50,"#"),"_",TEXT(B50,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_146_113_128_8</v>
       </c>
       <c r="I50" s="3" t="str">
@@ -3439,7 +3439,7 @@
         <v>2</v>
       </c>
       <c r="H51" s="3" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E51,"#"),"_",TEXT(C51,"#"),"_",TEXT(D51,"#"),"_",TEXT(B51,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_140_90_111_8</v>
       </c>
       <c r="I51" s="3" t="str">
@@ -3473,7 +3473,7 @@
         <v>2</v>
       </c>
       <c r="H52" s="11" t="str">
-        <f>_xlfn.CONCAT("C","_",TEXT(E52,"#"),"_",TEXT(C52,"#"),"_",TEXT(D52,"#"),"_",TEXT(B52,"#"))</f>
+        <f t="shared" si="1"/>
         <v>C_141_100_119_8</v>
       </c>
       <c r="I52" s="11" t="str">

</xml_diff>